<commit_message>
fix(WordPackManagement): fix wordpack library file example missing; fix upload result error handle
</commit_message>
<xml_diff>
--- a/public/recommended-packs/standard-japanese-junior.xlsx
+++ b/public/recommended-packs/standard-japanese-junior.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sone/Desktop/tango/public/recommended-packs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8EE553-529D-0440-BBDE-E1C3C5CA3574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C43270-E6CB-F041-AB77-70D178FCD694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8641" uniqueCount="6335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8642" uniqueCount="6335">
   <si>
     <t>音标</t>
   </si>
@@ -19448,8 +19448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0050C82-831D-7C47-A19C-0DC06CBA004F}">
   <dimension ref="A1:G2143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1333" workbookViewId="0">
-      <selection activeCell="C1369" sqref="C1369"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19472,7 +19472,9 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4"/>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>

</xml_diff>